<commit_message>
Processes crbeCountries manytomany relation added
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/ivp.xlsx
+++ b/storage/app/excel/templates/ivp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DB05BF-2E25-43FE-A111-3989D913316A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447280A6-F86F-4754-BAB0-194ED3A01F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     <t>Срок годности</t>
   </si>
   <si>
-    <t>Срок дейст. патента</t>
+    <t>Срок дейст.</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +528,7 @@
     <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" style="1" customWidth="1"/>
     <col min="19" max="19" width="11.85546875" style="1" customWidth="1"/>

</xml_diff>